<commit_message>
perbaiki tabel produk dan report pesanan
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,45 +15,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+  <si>
+    <t>Nama Penerima</t>
+  </si>
+  <si>
+    <t>Agung Tri Saputra</t>
+  </si>
+  <si>
+    <t>Nomor WA</t>
+  </si>
+  <si>
+    <t>081328907767</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>Kost Indah Jaya Belakang No. 19, Jl. Medan Baru VI, Kandang Limun, Bengkulu</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Barang Pesanan</t>
+  </si>
+  <si>
+    <t>No Lokasi</t>
+  </si>
+  <si>
+    <t>No Urut</t>
+  </si>
   <si>
     <t>Nama Produk</t>
   </si>
   <si>
-    <t>Harga</t>
+    <t>Harga (RP)</t>
   </si>
   <si>
     <t>Jumlah</t>
   </si>
   <si>
-    <t>Sub Total</t>
+    <t>Sub Total (RP)</t>
   </si>
   <si>
     <t>Tomat</t>
   </si>
   <si>
-    <t>Rp10.000,00</t>
-  </si>
-  <si>
-    <t>Rp30.000,00</t>
+    <t>10.000,00</t>
+  </si>
+  <si>
+    <t>30.000,00</t>
   </si>
   <si>
     <t>Brokoli</t>
   </si>
   <si>
-    <t>Rp31.000,00</t>
+    <t>31.000,00</t>
   </si>
   <si>
     <t>Wortel</t>
   </si>
   <si>
-    <t>Rp12.000,00</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Rp73.000,00</t>
+    <t>12.000,00</t>
+  </si>
+  <si>
+    <t>TOTAL (RP)</t>
+  </si>
+  <si>
+    <t>73.000,00</t>
   </si>
 </sst>
 </file>
@@ -61,9 +91,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -83,17 +122,43 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -395,90 +460,175 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="A9" sqref="A9:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="15" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18" customWidth="true" style="0"/>
+    <col min="3" max="3" width="18" customWidth="true" style="0"/>
+    <col min="4" max="4" width="12" customWidth="true" style="0"/>
+    <col min="5" max="5" width="8" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
+      <c r="F11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
+      <c r="F12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="F13" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A14:E14"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ubah format report dan tabel product
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,69 +15,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
-  <si>
-    <t>Nama Penerima</t>
-  </si>
-  <si>
-    <t>Agung Tri Saputra</t>
-  </si>
-  <si>
-    <t>Nomor WA</t>
-  </si>
-  <si>
-    <t>081328907767</t>
-  </si>
-  <si>
-    <t>Alamat</t>
-  </si>
-  <si>
-    <t>Kost Indah Jaya Belakang No. 19, Jl. Medan Baru VI, Kandang Limun, Bengkulu</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Barang Pesanan</t>
   </si>
   <si>
-    <t>No Lokasi</t>
-  </si>
-  <si>
-    <t>No Urut</t>
-  </si>
-  <si>
-    <t>Nama Produk</t>
-  </si>
-  <si>
-    <t>Harga (RP)</t>
+    <t>Harga Real</t>
+  </si>
+  <si>
+    <t>Harga Beli/kg (Rp)</t>
   </si>
   <si>
     <t>Jumlah</t>
   </si>
   <si>
-    <t>Sub Total (RP)</t>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Kategori</t>
+  </si>
+  <si>
+    <t>Pembeli</t>
+  </si>
+  <si>
+    <t>Penjual</t>
+  </si>
+  <si>
+    <t>No. Hp</t>
+  </si>
+  <si>
+    <t>Lokasi</t>
+  </si>
+  <si>
+    <t>Sub Total</t>
+  </si>
+  <si>
+    <t>10.000,00</t>
   </si>
   <si>
     <t>Tomat</t>
   </si>
   <si>
-    <t>10.000,00</t>
+    <t>Sayur</t>
   </si>
   <si>
     <t>30.000,00</t>
   </si>
   <si>
+    <t>31.000,00</t>
+  </si>
+  <si>
     <t>Brokoli</t>
   </si>
   <si>
-    <t>31.000,00</t>
+    <t>12.000,00</t>
   </si>
   <si>
     <t>Wortel</t>
-  </si>
-  <si>
-    <t>12.000,00</t>
   </si>
   <si>
     <t>TOTAL (RP)</t>
@@ -142,18 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -460,10 +445,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A9" sqref="A9:F14"/>
+      <selection activeCell="A1" sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -476,159 +461,139 @@
     <col min="6" max="6" width="15" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
         <v>3</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="5">
-        <v>3</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:I6"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>